<commit_message>
scraping completo. falta comprobar version de chrome
</commit_message>
<xml_diff>
--- a/instagram.xlsx
+++ b/instagram.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barrio\Desktop\Desarrollo\Proyectos\instagram_scrapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barrio\Desktop\Desarrollo\Proyectos\instagram_scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1649FA-09E6-42D4-8900-6D87D322D9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7569F1DF-5642-44B9-A462-CDE3765015E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0644A942-00E5-4874-A21B-3AB26CD65544}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="90">
   <si>
     <t>https://www.instagram.com/la_historia_es_meme/</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>Historia (NO TIENE POSTS EN 2022)</t>
+  </si>
+  <si>
+    <t>Historia (PUBLICACIÓN OCULTA)</t>
   </si>
 </sst>
 </file>
@@ -744,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F1AE70-FAE6-44F1-A4DC-634D8084CD80}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1302,7 @@
         <v>9304</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>2</v>

</xml_diff>